<commit_message>
added second and third level
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
   <si>
     <t>H</t>
   </si>
@@ -66,13 +66,25 @@
   </si>
   <si>
     <t>Wall</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Falling rock</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +96,13 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -164,6 +183,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:AZ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AV16" sqref="AV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,21 +482,29 @@
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:52" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AT2" s="2"/>
+      <c r="AZ2" s="2"/>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -486,8 +516,26 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AZ3" s="2"/>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -496,28 +544,95 @@
       <c r="E4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AM4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT4" s="2"/>
+      <c r="AZ4" s="2"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2"/>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AZ5" s="2"/>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T6" s="2"/>
+      <c r="U6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="5"/>
+      <c r="AN6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ6" s="2"/>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,8 +646,21 @@
       <c r="L7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T7" s="2"/>
+      <c r="V7" s="4"/>
+      <c r="Z7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2"/>
+      <c r="AC7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AZ7" s="2"/>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -545,8 +673,28 @@
       </c>
       <c r="L8" s="4"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AE8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AN8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="2"/>
+      <c r="AZ8" s="2"/>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -560,8 +708,30 @@
       </c>
       <c r="L9" s="2"/>
       <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AH9" s="8"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AZ9" s="2"/>
+    </row>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="K10" s="2"/>
@@ -570,8 +740,23 @@
         <v>0</v>
       </c>
       <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AC10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -579,15 +764,31 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+    </row>
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="Y12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="2"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E13" s="2"/>
       <c r="H13" s="1" t="s">
         <v>0</v>
@@ -597,16 +798,39 @@
         <v>1</v>
       </c>
       <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="2"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="4"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="T14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="X14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
         <v>1</v>
@@ -618,8 +842,21 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
@@ -631,8 +868,17 @@
         <v>0</v>
       </c>
       <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD16" s="2"/>
+    </row>
+    <row r="17" spans="4:30" x14ac:dyDescent="0.3">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="I17" s="2"/>
@@ -640,8 +886,17 @@
       <c r="K17" s="2"/>
       <c r="N17" s="2"/>
       <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R17" s="2"/>
+      <c r="S17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="2"/>
+    </row>
+    <row r="18" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -651,16 +906,35 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R18" s="2"/>
+      <c r="W18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="2"/>
+    </row>
+    <row r="19" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D19" s="2"/>
       <c r="H19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="2"/>
       <c r="P19" s="2"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R19" s="7">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="2"/>
+    </row>
+    <row r="20" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1" t="s">
@@ -672,8 +946,15 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AD20" s="2"/>
+    </row>
+    <row r="21" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -683,19 +964,47 @@
       <c r="K21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AD21" s="2"/>
+    </row>
+    <row r="22" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D22" s="2"/>
       <c r="F22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R22" s="2"/>
+      <c r="T22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD22" s="2"/>
+    </row>
+    <row r="23" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
       <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R23" s="2"/>
+      <c r="AD23" s="2"/>
+    </row>
+    <row r="24" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -705,28 +1014,98 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R24" s="2"/>
+      <c r="AD24" s="2"/>
+    </row>
+    <row r="25" spans="4:30" x14ac:dyDescent="0.3">
       <c r="G25" s="2"/>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+    </row>
+    <row r="26" spans="4:30" x14ac:dyDescent="0.3">
       <c r="G26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AC26" s="2"/>
+    </row>
+    <row r="27" spans="4:30" x14ac:dyDescent="0.3">
       <c r="G27" s="2"/>
       <c r="I27" s="5"/>
       <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="S27" s="2"/>
+      <c r="V27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="4:30" x14ac:dyDescent="0.3">
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="AC28" s="2"/>
+    </row>
+    <row r="29" spans="4:30" x14ac:dyDescent="0.3">
+      <c r="S29" s="2"/>
+      <c r="AC29" s="2"/>
+    </row>
+    <row r="30" spans="4:30" x14ac:dyDescent="0.3">
+      <c r="S30" s="2"/>
+      <c r="AC30" s="2"/>
+    </row>
+    <row r="31" spans="4:30" x14ac:dyDescent="0.3">
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+    </row>
+    <row r="32" spans="4:30" x14ac:dyDescent="0.3">
+      <c r="S32" s="2"/>
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="19:23" x14ac:dyDescent="0.3">
+      <c r="S33" s="2"/>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="19:23" x14ac:dyDescent="0.3">
+      <c r="S34" s="2"/>
+      <c r="U34" s="5"/>
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="19:23" x14ac:dyDescent="0.3">
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added player sprite and movement
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>